<commit_message>
fixed grammatical errors in BP xl
</commit_message>
<xml_diff>
--- a/BusinessPlanExcel.xlsx
+++ b/BusinessPlanExcel.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16828"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app\GIP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maksim.superfin\Documents\GIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="profit" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="comission plan" sheetId="5" r:id="rId5"/>
     <sheet name="investors" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,9 +34,6 @@
     <t>Profit</t>
   </si>
   <si>
-    <t>Expensies</t>
-  </si>
-  <si>
     <t>Investments</t>
   </si>
   <si>
@@ -169,9 +166,6 @@
     <t>Ratio of north america</t>
   </si>
   <si>
-    <t>Customers in north america</t>
-  </si>
-  <si>
     <t>USD</t>
   </si>
   <si>
@@ -289,9 +283,6 @@
     <t>Number of current customers</t>
   </si>
   <si>
-    <t>Avarege comission per purchise</t>
-  </si>
-  <si>
     <t>Revenue from Current customers</t>
   </si>
   <si>
@@ -307,9 +298,6 @@
     <t>Revenue from Potential customers</t>
   </si>
   <si>
-    <t>Table 1. Revenue per progect in 3 years period of time</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 1 YEAR</t>
   </si>
   <si>
@@ -328,9 +316,6 @@
     <t xml:space="preserve">Annual revenue </t>
   </si>
   <si>
-    <t>Number og Grupon subscribers (quaterly)</t>
-  </si>
-  <si>
     <t>142.87 m</t>
   </si>
   <si>
@@ -338,13 +323,28 @@
   </si>
   <si>
     <t>Global Revenue of Groupon</t>
+  </si>
+  <si>
+    <t>Table 1. Revenue per project in 3 years period of time</t>
+  </si>
+  <si>
+    <t>Avarege comission per purchase</t>
+  </si>
+  <si>
+    <t>Customers in North America</t>
+  </si>
+  <si>
+    <t>Number of Grupon subscribers (quaterly)</t>
+  </si>
+  <si>
+    <t>Expenses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -405,6 +405,13 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -499,7 +506,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -560,6 +567,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,7 +586,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -592,6 +600,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -770,7 +779,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-39AF-4AC5-9F78-8C8C93F1F675}"/>
             </c:ext>
@@ -786,9 +795,9 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="408969176"/>
-        <c:axId val="408967536"/>
-        <c:extLst>
+        <c:axId val="283290760"/>
+        <c:axId val="283292720"/>
+        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
               <c15:ser>
@@ -796,7 +805,7 @@
                 <c:order val="0"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'revenue&amp;graphs'!$S$6</c15:sqref>
@@ -852,7 +861,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'revenue&amp;graphs'!$T$5:$AE$5</c15:sqref>
@@ -902,7 +911,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'revenue&amp;graphs'!$T$6:$AE$6</c15:sqref>
@@ -951,7 +960,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000000-39AF-4AC5-9F78-8C8C93F1F675}"/>
                   </c:ext>
@@ -962,7 +971,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="408969176"/>
+        <c:axId val="283290760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1005,7 +1014,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408967536"/>
+        <c:crossAx val="283292720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1013,7 +1022,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="408967536"/>
+        <c:axId val="283292720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1064,7 +1073,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="408969176"/>
+        <c:crossAx val="283290760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1078,6 +1087,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1145,7 +1155,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1159,6 +1169,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1337,7 +1348,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-09C9-4B90-ADEE-571462810A8F}"/>
             </c:ext>
@@ -1353,11 +1364,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="402960968"/>
-        <c:axId val="402959328"/>
+        <c:axId val="283293896"/>
+        <c:axId val="283295072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="402960968"/>
+        <c:axId val="283293896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1400,7 +1411,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="402959328"/>
+        <c:crossAx val="283295072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1408,7 +1419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="402959328"/>
+        <c:axId val="283295072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1459,7 +1470,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="402960968"/>
+        <c:crossAx val="283293896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1509,7 +1520,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1523,6 +1534,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1701,7 +1713,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-51F9-4B50-A16F-6CA11207665B}"/>
             </c:ext>
@@ -1717,11 +1729,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="374828520"/>
-        <c:axId val="374828848"/>
+        <c:axId val="283296248"/>
+        <c:axId val="283288800"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="374828520"/>
+        <c:axId val="283296248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1764,7 +1776,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374828848"/>
+        <c:crossAx val="283288800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1772,7 +1784,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="374828848"/>
+        <c:axId val="283288800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1823,7 +1835,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="374828520"/>
+        <c:crossAx val="283296248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1873,7 +1885,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1887,6 +1899,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2011,7 +2024,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-274F-4DE3-89E1-383BFB4885F7}"/>
             </c:ext>
@@ -2027,11 +2040,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="387687384"/>
-        <c:axId val="387685744"/>
+        <c:axId val="283293112"/>
+        <c:axId val="283291544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="387687384"/>
+        <c:axId val="283293112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2074,7 +2087,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387685744"/>
+        <c:crossAx val="283291544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2082,7 +2095,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="387685744"/>
+        <c:axId val="283291544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2133,7 +2146,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="387687384"/>
+        <c:crossAx val="283293112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2183,7 +2196,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2197,6 +2210,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2228,7 +2242,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.14992871809417482"/>
+          <c:y val="2.5428331875182269E-2"/>
+          <c:w val="0.80286749092105236"/>
+          <c:h val="0.65873468941382329"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -2375,7 +2399,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-CD53-465D-8CA8-784AA303CC8B}"/>
             </c:ext>
@@ -2391,11 +2415,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="384723200"/>
-        <c:axId val="384725168"/>
+        <c:axId val="283292328"/>
+        <c:axId val="283293504"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="384723200"/>
+        <c:axId val="283292328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2438,7 +2462,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384725168"/>
+        <c:crossAx val="283293504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2446,7 +2470,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="384725168"/>
+        <c:axId val="283293504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2497,7 +2521,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="384723200"/>
+        <c:crossAx val="283292328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5456,15 +5480,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>838200</xdr:colOff>
+      <xdr:colOff>143435</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>178174</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
+      <xdr:colOff>105335</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>63874</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5545,16 +5569,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>709333</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>45384</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>28</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>128307</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>121584</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5875,8 +5899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:R23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5897,20 +5921,20 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F4" t="s">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
         <v>3</v>
       </c>
-      <c r="K4" t="s">
+      <c r="P4" t="s">
         <v>4</v>
-      </c>
-      <c r="P4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="17">
+        <v>1</v>
+      </c>
+      <c r="F7" s="32">
         <v>750000</v>
       </c>
       <c r="G7" s="17"/>
@@ -5954,7 +5978,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F10" s="17">
         <f>'revenue&amp;graphs'!V59</f>
@@ -6027,7 +6051,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
@@ -6149,7 +6173,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -6169,18 +6193,18 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C2">
         <v>2.99</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -6192,8 +6216,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AH67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB57" sqref="AB57"/>
+    <sheetView topLeftCell="A40" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6214,56 +6238,56 @@
   <sheetData>
     <row r="2" spans="11:34" x14ac:dyDescent="0.25">
       <c r="K2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="11:34" x14ac:dyDescent="0.25">
       <c r="S4" s="14" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="11:34" x14ac:dyDescent="0.25">
       <c r="S5" s="20"/>
       <c r="T5" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="U5" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="V5" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="W5" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="V5" s="21" t="s">
+      <c r="X5" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y5" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="W5" s="21" t="s">
+      <c r="Z5" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="X5" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y5" s="21" t="s">
+      <c r="AA5" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="Z5" s="21" t="s">
+      <c r="AB5" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC5" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="AA5" s="21" t="s">
+      <c r="AD5" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="AB5" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="AC5" s="21" t="s">
+      <c r="AE5" s="21" t="s">
         <v>81</v>
-      </c>
-      <c r="AD5" s="21" t="s">
-        <v>82</v>
-      </c>
-      <c r="AE5" s="21" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="6" spans="11:34" x14ac:dyDescent="0.25">
       <c r="S6" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="T6" s="29">
         <v>0.01</v>
@@ -6313,12 +6337,12 @@
         <v>0.69</v>
       </c>
       <c r="AH6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="11:34" x14ac:dyDescent="0.25">
       <c r="S7" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="T7" s="22">
         <f>$N$45*T6</f>
@@ -6369,7 +6393,7 @@
         <v>21740307.692307692</v>
       </c>
       <c r="AG7" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="AH7" s="17">
         <f>W14</f>
@@ -6378,7 +6402,7 @@
     </row>
     <row r="8" spans="11:34" x14ac:dyDescent="0.25">
       <c r="S8" s="20" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="T8" s="20">
         <f>P49</f>
@@ -6429,7 +6453,7 @@
         <v>0.65</v>
       </c>
       <c r="AG8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="AH8" s="17">
         <f>AA14</f>
@@ -6438,7 +6462,7 @@
     </row>
     <row r="9" spans="11:34" x14ac:dyDescent="0.25">
       <c r="S9" s="20" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="T9" s="23">
         <f>T8*T7</f>
@@ -6489,7 +6513,7 @@
         <v>14131200</v>
       </c>
       <c r="AG9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="AH9" s="17">
         <f>AE14</f>
@@ -6498,7 +6522,7 @@
     </row>
     <row r="10" spans="11:34" x14ac:dyDescent="0.25">
       <c r="S10" s="20" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="T10" s="29">
         <v>0.01</v>
@@ -6554,7 +6578,7 @@
     </row>
     <row r="11" spans="11:34" x14ac:dyDescent="0.25">
       <c r="S11" s="20" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="T11" s="22">
         <f>$P$54*T10</f>
@@ -6608,7 +6632,7 @@
     </row>
     <row r="12" spans="11:34" ht="15.75" x14ac:dyDescent="0.25">
       <c r="S12" s="20" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="T12" s="23">
         <f>T8*0.1</f>
@@ -6659,12 +6683,12 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="AG12" s="30" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="11:34" x14ac:dyDescent="0.25">
       <c r="S13" s="20" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="T13" s="23">
         <v>57520</v>
@@ -6703,7 +6727,7 @@
         <v>1754360.0000000002</v>
       </c>
       <c r="AG13" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="AH13">
         <f>((AH8-AH7)/AH7+(AH9-AH8)/AH8)/2</f>
@@ -6712,7 +6736,7 @@
     </row>
     <row r="14" spans="11:34" s="14" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="S14" s="24" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="T14" s="25"/>
       <c r="U14" s="25"/>
@@ -6750,12 +6774,12 @@
         <v>120000000</v>
       </c>
       <c r="O32" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="9:30" x14ac:dyDescent="0.25">
       <c r="I34" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K34">
         <f>D32/N32</f>
@@ -6770,7 +6794,7 @@
     </row>
     <row r="39" spans="9:30" x14ac:dyDescent="0.25">
       <c r="L39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="40" spans="9:30" x14ac:dyDescent="0.25">
@@ -6778,7 +6802,7 @@
         <v>3120000000</v>
       </c>
       <c r="S40" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="T40">
         <v>0.02</v>
@@ -6797,45 +6821,45 @@
     </row>
     <row r="42" spans="9:30" x14ac:dyDescent="0.25">
       <c r="S42" t="s">
+        <v>50</v>
+      </c>
+      <c r="T42" t="s">
+        <v>51</v>
+      </c>
+      <c r="U42" t="s">
         <v>52</v>
       </c>
-      <c r="T42" t="s">
+      <c r="V42" t="s">
         <v>53</v>
       </c>
-      <c r="U42" t="s">
+      <c r="W42" t="s">
         <v>54</v>
       </c>
-      <c r="V42" t="s">
+      <c r="X42" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA42" t="s">
         <v>55</v>
       </c>
-      <c r="W42" t="s">
-        <v>56</v>
-      </c>
-      <c r="X42" t="s">
+      <c r="AB42" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD42" t="s">
         <v>53</v>
-      </c>
-      <c r="Y42" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z42" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA42" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB42" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC42" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD42" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="43" spans="9:30" x14ac:dyDescent="0.25">
       <c r="K43" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M43">
         <f>L41/L40</f>
@@ -6844,10 +6868,10 @@
     </row>
     <row r="44" spans="9:30" x14ac:dyDescent="0.25">
       <c r="O44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="R44" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="S44">
         <v>0.01</v>
@@ -6899,17 +6923,17 @@
     </row>
     <row r="45" spans="9:30" x14ac:dyDescent="0.25">
       <c r="L45" t="s">
-        <v>46</v>
+        <v>100</v>
       </c>
       <c r="N45" s="16">
         <f>K36*M43</f>
         <v>31507692.307692308</v>
       </c>
       <c r="O45" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="R45" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S45">
         <f>$N$45*S44</f>
@@ -6962,10 +6986,10 @@
     </row>
     <row r="46" spans="9:30" x14ac:dyDescent="0.25">
       <c r="O46" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R46" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="S46">
         <f>S45*$P$49</f>
@@ -7026,7 +7050,7 @@
         <v>1.9500000000000002</v>
       </c>
       <c r="R47" s="14" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="V47" s="14">
         <f>S46+T46+U46+V46</f>
@@ -7043,7 +7067,7 @@
     </row>
     <row r="49" spans="12:30" x14ac:dyDescent="0.25">
       <c r="N49" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P49" s="16">
         <f>P47/12*4</f>
@@ -7057,7 +7081,7 @@
       <c r="Q50" s="16"/>
       <c r="R50" s="16"/>
       <c r="S50" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="T50">
         <v>5.0000000000000001E-3</v>
@@ -7079,40 +7103,40 @@
       <c r="Q52" s="16"/>
       <c r="R52" s="16"/>
       <c r="S52" t="s">
+        <v>50</v>
+      </c>
+      <c r="T52" t="s">
+        <v>51</v>
+      </c>
+      <c r="U52" t="s">
         <v>52</v>
       </c>
-      <c r="T52" t="s">
+      <c r="V52" t="s">
         <v>53</v>
       </c>
-      <c r="U52" t="s">
+      <c r="W52" t="s">
         <v>54</v>
       </c>
-      <c r="V52" t="s">
+      <c r="X52" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA52" t="s">
         <v>55</v>
       </c>
-      <c r="W52" t="s">
-        <v>56</v>
-      </c>
-      <c r="X52" t="s">
+      <c r="AB52" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC52" t="s">
+        <v>52</v>
+      </c>
+      <c r="AD52" t="s">
         <v>53</v>
-      </c>
-      <c r="Y52" t="s">
-        <v>54</v>
-      </c>
-      <c r="Z52" t="s">
-        <v>55</v>
-      </c>
-      <c r="AA52" t="s">
-        <v>57</v>
-      </c>
-      <c r="AB52" t="s">
-        <v>53</v>
-      </c>
-      <c r="AC52" t="s">
-        <v>54</v>
-      </c>
-      <c r="AD52" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="53" spans="12:30" x14ac:dyDescent="0.25">
@@ -7122,14 +7146,14 @@
     </row>
     <row r="54" spans="12:30" x14ac:dyDescent="0.25">
       <c r="L54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="P54">
         <f>N32-N45</f>
         <v>88492307.692307696</v>
       </c>
       <c r="R54" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="S54">
         <v>0.01</v>
@@ -7185,7 +7209,7 @@
         <v>6.5000000000000002E-2</v>
       </c>
       <c r="R55" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="S55">
         <f>$P$54*S54</f>
@@ -7238,7 +7262,7 @@
     </row>
     <row r="56" spans="12:30" x14ac:dyDescent="0.25">
       <c r="R56" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="S56">
         <f>S55*$P$55</f>
@@ -7291,7 +7315,7 @@
     </row>
     <row r="57" spans="12:30" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R57" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="V57" s="14">
         <f>S56+T56+U56+V56</f>
@@ -7308,7 +7332,7 @@
     </row>
     <row r="59" spans="12:30" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="R59" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="V59" s="18">
         <f>SUM(V47,V57)</f>
@@ -7325,13 +7349,13 @@
     </row>
     <row r="61" spans="12:30" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="N61" s="14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P61" s="18">
         <v>750000</v>
       </c>
       <c r="R61" s="14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="V61" s="19">
         <f>V59/P61</f>
@@ -7348,18 +7372,18 @@
     </row>
     <row r="66" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G66" s="31" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G67" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -7373,9 +7397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
+    <sheetView topLeftCell="A25" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -7387,7 +7409,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -7395,21 +7417,21 @@
     </row>
     <row r="2" spans="1:8" ht="63.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="7">
         <v>0.05</v>
@@ -7423,7 +7445,7 @@
     </row>
     <row r="4" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" s="12">
         <v>0.05</v>
@@ -7437,7 +7459,7 @@
     </row>
     <row r="5" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" s="7">
         <v>0.05</v>
@@ -7451,7 +7473,7 @@
     </row>
     <row r="6" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="7">
         <v>0.05</v>
@@ -7465,7 +7487,7 @@
     </row>
     <row r="7" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="7">
         <v>0.05</v>
@@ -7479,7 +7501,7 @@
     </row>
     <row r="8" spans="1:8" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B8" s="7">
         <v>0.05</v>
@@ -7497,7 +7519,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="7">
         <v>0.05</v>
@@ -7515,7 +7537,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="7">
         <v>0.05</v>
@@ -7533,7 +7555,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="7">
         <v>0.05</v>
@@ -7547,7 +7569,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B12" s="7">
         <v>0.05</v>
@@ -7561,7 +7583,7 @@
     </row>
     <row r="13" spans="1:8" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="15">
         <v>2.5000000000000001E-2</v>
@@ -7575,7 +7597,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B14" s="10">
         <v>2.5000000000000001E-2</v>
@@ -7589,7 +7611,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="10">
         <v>2.5000000000000001E-2</v>
@@ -7603,7 +7625,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="10">
         <v>2.5000000000000001E-2</v>
@@ -7617,7 +7639,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="10">
         <v>2.5000000000000001E-2</v>
@@ -7631,7 +7653,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="10">
         <v>2.5000000000000001E-2</v>
@@ -7645,7 +7667,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="10">
         <v>2.5000000000000001E-2</v>
@@ -7659,7 +7681,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="10">
         <v>2.5000000000000001E-2</v>
@@ -7673,7 +7695,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="10">
         <v>2.5000000000000001E-2</v>
@@ -7687,7 +7709,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="7">
         <v>0.05</v>
@@ -7701,7 +7723,7 @@
     </row>
     <row r="23" spans="1:4" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="12">
         <v>0.05</v>
@@ -7715,7 +7737,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="7">
         <v>0.05</v>
@@ -7729,7 +7751,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="7">
         <v>0.05</v>
@@ -7743,7 +7765,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="7">
         <v>0.05</v>
@@ -7757,7 +7779,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="7">
         <v>0.05</v>
@@ -7771,7 +7793,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28" s="7">
         <v>0.05</v>
@@ -7785,7 +7807,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B29" s="7">
         <v>0.05</v>
@@ -7799,7 +7821,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B30" s="7">
         <v>0.05</v>
@@ -7813,7 +7835,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B31" s="7">
         <v>0.05</v>
@@ -7827,7 +7849,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32" s="7">
         <v>0.05</v>
@@ -7841,7 +7863,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B33" s="7">
         <v>0.05</v>
@@ -7855,7 +7877,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="7">
         <v>0.05</v>
@@ -7869,7 +7891,7 @@
     </row>
     <row r="35" spans="1:4" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="7">
         <v>0</v>

</xml_diff>